<commit_message>
correcting the browser path
</commit_message>
<xml_diff>
--- a/DDT.xlsx
+++ b/DDT.xlsx
@@ -399,7 +399,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>

</xml_diff>